<commit_message>
continued with lab 11
</commit_message>
<xml_diff>
--- a/lab11/a2_1.xlsx
+++ b/lab11/a2_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\SEM7\kry\lab11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Workspace\ZHAW\SEM7\kry\lab11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00ACB5FA-E49F-4F91-995A-5D581ABAE9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9418B6D-D9E3-4015-852E-2E6F266FC8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="2640" windowWidth="22650" windowHeight="11925" xr2:uid="{E9810C01-AADD-4785-821B-D33B8496B9AA}"/>
+    <workbookView xWindow="1845" yWindow="825" windowWidth="26190" windowHeight="16635" xr2:uid="{E9810C01-AADD-4785-821B-D33B8496B9AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,13 +59,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,14 +98,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -103,7 +123,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -402,10 +422,10 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -501,47 +521,47 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="b">
+      <c r="B3" s="2" t="b">
         <f>MOD(B2^5,11)=1</f>
         <v>1</v>
       </c>
-      <c r="C3" t="b">
+      <c r="C3" s="3" t="b">
         <f t="shared" ref="C3:L3" si="1">MOD(C2^5,11)=1</f>
         <v>0</v>
       </c>
-      <c r="D3" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E3" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G3" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="H3" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I3" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="J3" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K3" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L3" t="b">
+      <c r="D3" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F3" s="2" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H3" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J3" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K3" s="3" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L3" s="3" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>